<commit_message>
Récupération données depuis excell - Récupération des produits commandé dans un dictionnaire
</commit_message>
<xml_diff>
--- a/Commandes.xlsx
+++ b/Commandes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2irs\Desktop\E5\RPA Expertise\Projet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2irs\Desktop\E5\RPA Expertise\Projet\AutomatisationGestionCommandes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1817259-70ED-4590-942A-75E92A857D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{304311D9-F1D3-40CF-8500-6B290EDDAFEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>Numéro de commande</t>
   </si>
@@ -78,9 +78,6 @@
     <t>Ordinateur portable</t>
   </si>
   <si>
-    <t>En cours de traitement</t>
-  </si>
-  <si>
     <t>David Johnson</t>
   </si>
   <si>
@@ -88,9 +85,6 @@
   </si>
   <si>
     <t>Casque audio Sony</t>
-  </si>
-  <si>
-    <t>Expédié</t>
   </si>
   <si>
     <t>Sarah Wilson</t>
@@ -430,7 +424,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,7 +528,7 @@
         <v>899.99</v>
       </c>
       <c r="H3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="I3" s="1">
         <v>45212</v>
@@ -548,13 +542,13 @@
         <v>1003</v>
       </c>
       <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -566,7 +560,7 @@
         <v>389.97</v>
       </c>
       <c r="H4" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="I4" s="1">
         <v>45213</v>
@@ -580,13 +574,13 @@
         <v>1004</v>
       </c>
       <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
         <v>22</v>
-      </c>
-      <c r="C5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" t="s">
-        <v>24</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -598,7 +592,7 @@
         <v>659.98</v>
       </c>
       <c r="H5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="I5" s="1">
         <v>45213</v>
@@ -612,13 +606,13 @@
         <v>1005</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -630,7 +624,7 @@
         <v>79.989999999999995</v>
       </c>
       <c r="H6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="I6" s="1">
         <v>45214</v>

</xml_diff>

<commit_message>
If Stock dispo alors réduction ok + expédié status ok
</commit_message>
<xml_diff>
--- a/Commandes.xlsx
+++ b/Commandes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2irs\Desktop\E5\RPA Expertise\Projet\AutomatisationGestionCommandes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{304311D9-F1D3-40CF-8500-6B290EDDAFEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96A0CCD4-35CA-4A5B-93ED-4D135AC39906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2640" yWindow="2640" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -423,8 +423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,7 +475,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1001</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -507,7 +507,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1002</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
@@ -539,7 +539,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1003</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>17</v>
@@ -571,7 +571,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>1004</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
@@ -603,7 +603,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>1005</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
Datatable pour récup les items a restock
</commit_message>
<xml_diff>
--- a/Commandes.xlsx
+++ b/Commandes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2irs\Desktop\E5\RPA Expertise\Projet\AutomatisationGestionCommandes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B44C1B8-E1AE-462E-9A54-E2FA0ADE61DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D0F9542-D052-436B-9F32-C7EAC5442871}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>Numéro de commande</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Smartphone Samsung</t>
   </si>
   <si>
-    <t>En attente</t>
-  </si>
-  <si>
     <t>Jane Smith</t>
   </si>
   <si>
@@ -103,6 +100,12 @@
   </si>
   <si>
     <t>Michael Brown</t>
+  </si>
+  <si>
+    <t>Expédié</t>
+  </si>
+  <si>
+    <t>Stock insuffisant</t>
   </si>
 </sst>
 </file>
@@ -423,7 +426,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
@@ -496,7 +499,7 @@
         <v>999.98</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="I2" s="1">
         <v>45211</v>
@@ -510,13 +513,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -528,7 +531,7 @@
         <v>899.99</v>
       </c>
       <c r="H3" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="I3" s="1">
         <v>45212</v>
@@ -542,13 +545,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
         <v>17</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>18</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -560,7 +563,7 @@
         <v>389.97</v>
       </c>
       <c r="H4" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="I4" s="1">
         <v>45213</v>
@@ -574,13 +577,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
         <v>20</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>21</v>
-      </c>
-      <c r="D5" t="s">
-        <v>22</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -592,7 +595,7 @@
         <v>659.98</v>
       </c>
       <c r="H5" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="I5" s="1">
         <v>45213</v>
@@ -606,13 +609,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -624,7 +627,7 @@
         <v>79.989999999999995</v>
       </c>
       <c r="H6" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="I6" s="1">
         <v>45214</v>

</xml_diff>

<commit_message>
passage de la data table stock need dans le nouveau workflow
</commit_message>
<xml_diff>
--- a/Commandes.xlsx
+++ b/Commandes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2irs\Desktop\E5\RPA Expertise\Projet\AutomatisationGestionCommandes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D0F9542-D052-436B-9F32-C7EAC5442871}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6495CBB2-2B9C-4C5E-AE92-85288FC0FD9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2640" yWindow="2640" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -563,7 +563,7 @@
         <v>389.97</v>
       </c>
       <c r="H4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I4" s="1">
         <v>45213</v>

</xml_diff>

<commit_message>
Envoie de mail avec un tableau récap des commandes
</commit_message>
<xml_diff>
--- a/Commandes.xlsx
+++ b/Commandes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2irs\Desktop\E5\RPA Expertise\Projet\AutomatisationGestionCommandes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD016BE-F6FC-4039-8143-94E28B9BFA4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{350C800D-7D94-441B-89D4-CA703F6C0CC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2985" yWindow="2985" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -426,8 +426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>